<commit_message>
Updated slides and assignment
</commit_message>
<xml_diff>
--- a/Code/Exercises/Group time ATT.xlsx
+++ b/Code/Exercises/Group time ATT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Difference-in-Differences/Code/Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9EADFA-D325-044C-8559-DCF152DAFF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822AF4C3-AC62-1A4D-9E05-5698F6F63971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="500" windowWidth="39880" windowHeight="28200" activeTab="1" xr2:uid="{2EE18137-9303-494C-8C32-9DE193BE7F81}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="32920" windowHeight="26240" xr2:uid="{2EE18137-9303-494C-8C32-9DE193BE7F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic ATT" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>ATT(1986,t)</t>
   </si>
@@ -142,6 +142,36 @@
   </si>
   <si>
     <t>SA</t>
+  </si>
+  <si>
+    <t>Remember: these are not DiD equations.  These are ATT. Only the DiD equation</t>
+  </si>
+  <si>
+    <t>uses baseline. The ATT (any causal terms) are with respect, not to the baseline,</t>
+  </si>
+  <si>
+    <t>but to the COUNTERFACTUAL.</t>
+  </si>
+  <si>
+    <t>For calculating ATT(1986), what weight did I use?  I used w_86 = 1/24</t>
+  </si>
+  <si>
+    <t>&lt;-- These ATT(g) summaries of underlying causal parmaeters all used equal weights -- just not the same equal weights.</t>
+  </si>
+  <si>
+    <t>Simple ATT is equally weighted average over all 60 ATT(g,t) causal parameters</t>
+  </si>
+  <si>
+    <t>FYI: the simple and group ATT --&gt; These are just "summaries" of the underlying causal effects</t>
+  </si>
+  <si>
+    <t>There is no one ATT.  There are many different ways we might summarize these same 60 causal parameters.</t>
+  </si>
+  <si>
+    <t>Simple is one: it uses equal weights</t>
+  </si>
+  <si>
+    <t>Group is a different one: it also uses equal weights (1/4) but only after weighting unequally weighted ATT(g) summarie</t>
   </si>
 </sst>
 </file>
@@ -369,13 +399,7 @@
   <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,12 +492,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,6 +501,18 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,561 +827,609 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B26958-D2FD-B340-96F0-C0F0E677AC3F}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="51" t="s">
+      <c r="B1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="38">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="36">
         <v>1980</v>
       </c>
-      <c r="B2" s="47">
-        <v>0</v>
-      </c>
-      <c r="C2" s="47">
-        <v>0</v>
-      </c>
-      <c r="D2" s="47">
-        <v>0</v>
-      </c>
-      <c r="E2" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="38">
+      <c r="B2" s="41">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41">
+        <v>0</v>
+      </c>
+      <c r="D2" s="41">
+        <v>0</v>
+      </c>
+      <c r="E2" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="36">
         <v>1981</v>
       </c>
-      <c r="B3" s="47">
-        <v>0</v>
-      </c>
-      <c r="C3" s="47">
-        <v>0</v>
-      </c>
-      <c r="D3" s="47">
-        <v>0</v>
-      </c>
-      <c r="E3" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="38">
+      <c r="B3" s="41">
+        <v>0</v>
+      </c>
+      <c r="C3" s="41">
+        <v>0</v>
+      </c>
+      <c r="D3" s="41">
+        <v>0</v>
+      </c>
+      <c r="E3" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="36">
         <v>1982</v>
       </c>
-      <c r="B4" s="47">
-        <v>0</v>
-      </c>
-      <c r="C4" s="47">
-        <v>0</v>
-      </c>
-      <c r="D4" s="47">
-        <v>0</v>
-      </c>
-      <c r="E4" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="38">
+      <c r="B4" s="41">
+        <v>0</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="41">
+        <v>0</v>
+      </c>
+      <c r="E4" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
         <v>1983</v>
       </c>
-      <c r="B5" s="47">
-        <v>0</v>
-      </c>
-      <c r="C5" s="47">
-        <v>0</v>
-      </c>
-      <c r="D5" s="47">
-        <v>0</v>
-      </c>
-      <c r="E5" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="38">
+      <c r="B5" s="41">
+        <v>0</v>
+      </c>
+      <c r="C5" s="41">
+        <v>0</v>
+      </c>
+      <c r="D5" s="41">
+        <v>0</v>
+      </c>
+      <c r="E5" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="36">
         <v>1984</v>
       </c>
-      <c r="B6" s="47">
-        <v>0</v>
-      </c>
-      <c r="C6" s="47">
-        <v>0</v>
-      </c>
-      <c r="D6" s="47">
-        <v>0</v>
-      </c>
-      <c r="E6" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+      <c r="B6" s="41">
+        <v>0</v>
+      </c>
+      <c r="C6" s="41">
+        <v>0</v>
+      </c>
+      <c r="D6" s="41">
+        <v>0</v>
+      </c>
+      <c r="E6" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
         <v>1985</v>
       </c>
-      <c r="B7" s="47">
-        <v>0</v>
-      </c>
-      <c r="C7" s="47">
-        <v>0</v>
-      </c>
-      <c r="D7" s="47">
-        <v>0</v>
-      </c>
-      <c r="E7" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="38">
+      <c r="B7" s="41">
+        <v>0</v>
+      </c>
+      <c r="C7" s="41">
+        <v>0</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="36">
         <v>1986</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <v>10</v>
       </c>
-      <c r="C8" s="47">
-        <v>0</v>
-      </c>
-      <c r="D8" s="47">
-        <v>0</v>
-      </c>
-      <c r="E8" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="38">
+      <c r="C8" s="41">
+        <v>0</v>
+      </c>
+      <c r="D8" s="41">
+        <v>0</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="36">
         <v>1987</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="30">
         <v>20</v>
       </c>
-      <c r="C9" s="47">
-        <v>0</v>
-      </c>
-      <c r="D9" s="47">
-        <v>0</v>
-      </c>
-      <c r="E9" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="38">
+      <c r="C9" s="41">
+        <v>0</v>
+      </c>
+      <c r="D9" s="41">
+        <v>0</v>
+      </c>
+      <c r="E9" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="36">
         <v>1988</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="30">
         <v>30</v>
       </c>
-      <c r="C10" s="47">
-        <v>0</v>
-      </c>
-      <c r="D10" s="47">
-        <v>0</v>
-      </c>
-      <c r="E10" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="38">
+      <c r="C10" s="41">
+        <v>0</v>
+      </c>
+      <c r="D10" s="41">
+        <v>0</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="36">
         <v>1989</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="30">
         <v>40</v>
       </c>
-      <c r="C11" s="47">
-        <v>0</v>
-      </c>
-      <c r="D11" s="47">
-        <v>0</v>
-      </c>
-      <c r="E11" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="38">
+      <c r="C11" s="41">
+        <v>0</v>
+      </c>
+      <c r="D11" s="41">
+        <v>0</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="36">
         <v>1990</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="30">
         <v>50</v>
       </c>
-      <c r="C12" s="47">
-        <v>0</v>
-      </c>
-      <c r="D12" s="47">
-        <v>0</v>
-      </c>
-      <c r="E12" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
+      <c r="C12" s="41">
+        <v>0</v>
+      </c>
+      <c r="D12" s="41">
+        <v>0</v>
+      </c>
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
         <v>1991</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="30">
         <v>60</v>
       </c>
-      <c r="C13" s="47">
-        <v>0</v>
-      </c>
-      <c r="D13" s="47">
-        <v>0</v>
-      </c>
-      <c r="E13" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="38">
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <v>0</v>
+      </c>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="36">
         <v>1992</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="30">
         <v>70</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="31">
         <v>8</v>
       </c>
-      <c r="D14" s="47">
-        <v>0</v>
-      </c>
-      <c r="E14" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="38">
+      <c r="D14" s="41">
+        <v>0</v>
+      </c>
+      <c r="E14" s="42">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="36">
         <v>1993</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="30">
         <v>80</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="32">
         <v>16</v>
       </c>
-      <c r="D15" s="47">
-        <v>0</v>
-      </c>
-      <c r="E15" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="38">
+      <c r="D15" s="41">
+        <v>0</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="36">
         <v>1994</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="30">
         <v>90</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="32">
         <v>24</v>
       </c>
-      <c r="D16" s="47">
-        <v>0</v>
-      </c>
-      <c r="E16" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="38">
+      <c r="D16" s="41">
+        <v>0</v>
+      </c>
+      <c r="E16" s="42">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="36">
         <v>1995</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="30">
         <v>100</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="32">
         <v>32</v>
       </c>
-      <c r="D17" s="47">
-        <v>0</v>
-      </c>
-      <c r="E17" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="38">
+      <c r="D17" s="41">
+        <v>0</v>
+      </c>
+      <c r="E17" s="42">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="36">
         <v>1996</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="30">
         <v>110</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="32">
         <v>40</v>
       </c>
-      <c r="D18" s="47">
-        <v>0</v>
-      </c>
-      <c r="E18" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+      <c r="D18" s="41">
+        <v>0</v>
+      </c>
+      <c r="E18" s="42">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36">
         <v>1997</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="30">
         <v>120</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="32">
         <v>48</v>
       </c>
-      <c r="D19" s="47">
-        <v>0</v>
-      </c>
-      <c r="E19" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="38">
+      <c r="D19" s="41">
+        <v>0</v>
+      </c>
+      <c r="E19" s="42">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="36">
         <v>1998</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="30">
         <v>130</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="32">
         <v>56</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="34">
         <v>6</v>
       </c>
-      <c r="E20" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="38">
+      <c r="E20" s="42">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="36">
         <v>1999</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="30">
         <v>140</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="32">
         <v>64</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="35">
         <v>12</v>
       </c>
-      <c r="E21" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="38">
+      <c r="E21" s="42">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="36">
         <v>2000</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="30">
         <v>150</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="32">
         <v>72</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D22" s="35">
         <v>18</v>
       </c>
-      <c r="E22" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="38">
+      <c r="E22" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="36">
         <v>2001</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="30">
         <v>160</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="32">
         <v>80</v>
       </c>
-      <c r="D23" s="37">
+      <c r="D23" s="35">
         <v>24</v>
       </c>
-      <c r="E23" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="38">
+      <c r="E23" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="36">
         <v>2002</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="30">
         <v>170</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="32">
         <v>88</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="35">
         <v>30</v>
       </c>
-      <c r="E24" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
+      <c r="E24" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36">
         <v>2003</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="30">
         <v>180</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="33">
         <v>96</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="35">
         <v>36</v>
       </c>
-      <c r="E25" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="38">
+      <c r="E25" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="36">
         <v>2004</v>
       </c>
-      <c r="B26" s="40">
+      <c r="B26" s="38">
         <v>190</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="38">
         <v>104</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="38">
         <v>42</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="38">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="38">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="36">
         <v>2005</v>
       </c>
-      <c r="B27" s="41">
+      <c r="B27" s="39">
         <v>200</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="39">
         <v>112</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="39">
         <v>48</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="38">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="36">
         <v>2006</v>
       </c>
-      <c r="B28" s="41">
+      <c r="B28" s="39">
         <v>210</v>
       </c>
-      <c r="C28" s="41">
+      <c r="C28" s="39">
         <v>120</v>
       </c>
-      <c r="D28" s="41">
+      <c r="D28" s="39">
         <v>54</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="39">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="38">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="36">
         <v>2007</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="39">
         <v>220</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="39">
         <v>128</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="39">
         <v>60</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="38">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="36">
         <v>2008</v>
       </c>
-      <c r="B30" s="41">
+      <c r="B30" s="39">
         <v>230</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="39">
         <v>136</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="39">
         <v>66</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="39">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+    <row r="31" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="37">
         <v>2009</v>
       </c>
-      <c r="B31" s="42">
+      <c r="B31" s="40">
         <v>240</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="40">
         <v>144</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="40">
         <v>72</v>
       </c>
-      <c r="E31" s="42">
+      <c r="E31" s="40">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+    <row r="32" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="46"/>
+      <c r="B32" s="51">
+        <f>AVERAGE(B8:B31)</f>
+        <v>125</v>
+      </c>
+      <c r="C32" s="52">
+        <f>AVERAGE(C14:C31)</f>
+        <v>76</v>
+      </c>
+      <c r="D32" s="52">
+        <f>AVERAGE(D20:D31)</f>
+        <v>39</v>
+      </c>
+      <c r="E32" s="53">
+        <f>AVERAGE(E26:E31)</f>
+        <v>14</v>
+      </c>
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="3">
+        <f>AVERAGE(B8:B31,C14:C31,D20:D31,E26:E31)</f>
+        <v>82</v>
+      </c>
     </row>
     <row r="34" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="2">
+        <f>AVERAGE(B32:E32)</f>
+        <v>63.5</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
@@ -1368,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8FA5D0-DE9F-6548-A74E-2E4FC95C5DFC}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1379,661 +1457,661 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="51" t="s">
+      <c r="B1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="47" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="38">
+      <c r="A2" s="36">
         <v>1980</v>
       </c>
-      <c r="B2" s="47">
-        <v>0</v>
-      </c>
-      <c r="C2" s="47">
-        <v>0</v>
-      </c>
-      <c r="D2" s="47">
-        <v>0</v>
-      </c>
-      <c r="E2" s="48">
-        <v>0</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="B2" s="41">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41">
+        <v>0</v>
+      </c>
+      <c r="D2" s="41">
+        <v>0</v>
+      </c>
+      <c r="E2" s="42">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="38">
+      <c r="A3" s="36">
         <v>1981</v>
       </c>
-      <c r="B3" s="47">
-        <v>0</v>
-      </c>
-      <c r="C3" s="47">
-        <v>0</v>
-      </c>
-      <c r="D3" s="47">
-        <v>0</v>
-      </c>
-      <c r="E3" s="48">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="B3" s="41">
+        <v>0</v>
+      </c>
+      <c r="C3" s="41">
+        <v>0</v>
+      </c>
+      <c r="D3" s="41">
+        <v>0</v>
+      </c>
+      <c r="E3" s="42">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
+      <c r="A4" s="36">
         <v>1982</v>
       </c>
-      <c r="B4" s="47">
-        <v>0</v>
-      </c>
-      <c r="C4" s="47">
-        <v>0</v>
-      </c>
-      <c r="D4" s="47">
-        <v>0</v>
-      </c>
-      <c r="E4" s="48">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="B4" s="41">
+        <v>0</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="41">
+        <v>0</v>
+      </c>
+      <c r="E4" s="42">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="38">
+      <c r="A5" s="36">
         <v>1983</v>
       </c>
-      <c r="B5" s="47">
-        <v>0</v>
-      </c>
-      <c r="C5" s="47">
-        <v>0</v>
-      </c>
-      <c r="D5" s="47">
-        <v>0</v>
-      </c>
-      <c r="E5" s="48">
-        <v>0</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="B5" s="41">
+        <v>0</v>
+      </c>
+      <c r="C5" s="41">
+        <v>0</v>
+      </c>
+      <c r="D5" s="41">
+        <v>0</v>
+      </c>
+      <c r="E5" s="42">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="38">
+      <c r="A6" s="36">
         <v>1984</v>
       </c>
-      <c r="B6" s="47">
-        <v>0</v>
-      </c>
-      <c r="C6" s="47">
-        <v>0</v>
-      </c>
-      <c r="D6" s="47">
-        <v>0</v>
-      </c>
-      <c r="E6" s="48">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="B6" s="41">
+        <v>0</v>
+      </c>
+      <c r="C6" s="41">
+        <v>0</v>
+      </c>
+      <c r="D6" s="41">
+        <v>0</v>
+      </c>
+      <c r="E6" s="42">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+      <c r="A7" s="36">
         <v>1985</v>
       </c>
-      <c r="B7" s="47">
-        <v>0</v>
-      </c>
-      <c r="C7" s="47">
-        <v>0</v>
-      </c>
-      <c r="D7" s="47">
-        <v>0</v>
-      </c>
-      <c r="E7" s="48">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="B7" s="41">
+        <v>0</v>
+      </c>
+      <c r="C7" s="41">
+        <v>0</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="38">
+      <c r="A8" s="36">
         <v>1986</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <v>10</v>
       </c>
-      <c r="C8" s="47">
-        <v>0</v>
-      </c>
-      <c r="D8" s="47">
-        <v>0</v>
-      </c>
-      <c r="E8" s="48">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="C8" s="41">
+        <v>0</v>
+      </c>
+      <c r="D8" s="41">
+        <v>0</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="38">
+      <c r="A9" s="36">
         <v>1987</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="30">
         <v>20</v>
       </c>
-      <c r="C9" s="47">
-        <v>0</v>
-      </c>
-      <c r="D9" s="47">
-        <v>0</v>
-      </c>
-      <c r="E9" s="48">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="C9" s="41">
+        <v>0</v>
+      </c>
+      <c r="D9" s="41">
+        <v>0</v>
+      </c>
+      <c r="E9" s="42">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
+      <c r="A10" s="36">
         <v>1988</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="30">
         <v>30</v>
       </c>
-      <c r="C10" s="47">
-        <v>0</v>
-      </c>
-      <c r="D10" s="47">
-        <v>0</v>
-      </c>
-      <c r="E10" s="48">
-        <v>0</v>
-      </c>
-      <c r="H10" s="15" t="s">
+      <c r="C10" s="41">
+        <v>0</v>
+      </c>
+      <c r="D10" s="41">
+        <v>0</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="38">
+      <c r="A11" s="36">
         <v>1989</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="30">
         <v>40</v>
       </c>
-      <c r="C11" s="47">
-        <v>0</v>
-      </c>
-      <c r="D11" s="47">
-        <v>0</v>
-      </c>
-      <c r="E11" s="48">
-        <v>0</v>
-      </c>
-      <c r="H11" s="19" t="s">
+      <c r="C11" s="41">
+        <v>0</v>
+      </c>
+      <c r="D11" s="41">
+        <v>0</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="38">
+      <c r="A12" s="36">
         <v>1990</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="30">
         <v>50</v>
       </c>
-      <c r="C12" s="47">
-        <v>0</v>
-      </c>
-      <c r="D12" s="47">
-        <v>0</v>
-      </c>
-      <c r="E12" s="48">
-        <v>0</v>
-      </c>
-      <c r="H12" s="21" t="s">
+      <c r="C12" s="41">
+        <v>0</v>
+      </c>
+      <c r="D12" s="41">
+        <v>0</v>
+      </c>
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+      <c r="H12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
+      <c r="A13" s="36">
         <v>1991</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="30">
         <v>60</v>
       </c>
-      <c r="C13" s="47">
-        <v>0</v>
-      </c>
-      <c r="D13" s="47">
-        <v>0</v>
-      </c>
-      <c r="E13" s="48">
-        <v>0</v>
-      </c>
-      <c r="H13" s="21" t="s">
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <v>0</v>
+      </c>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="38">
+      <c r="A14" s="36">
         <v>1992</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="30">
         <v>70</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="31">
         <v>8</v>
       </c>
-      <c r="D14" s="47">
-        <v>0</v>
-      </c>
-      <c r="E14" s="48">
-        <v>0</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="D14" s="41">
+        <v>0</v>
+      </c>
+      <c r="E14" s="42">
+        <v>0</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="38">
+      <c r="A15" s="36">
         <v>1993</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="30">
         <v>80</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="32">
         <v>16</v>
       </c>
-      <c r="D15" s="47">
-        <v>0</v>
-      </c>
-      <c r="E15" s="48">
-        <v>0</v>
-      </c>
-      <c r="H15" s="21" t="s">
+      <c r="D15" s="41">
+        <v>0</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
+      <c r="A16" s="36">
         <v>1994</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="30">
         <v>90</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="32">
         <v>24</v>
       </c>
-      <c r="D16" s="47">
-        <v>0</v>
-      </c>
-      <c r="E16" s="48">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23" t="s">
+      <c r="D16" s="41">
+        <v>0</v>
+      </c>
+      <c r="E16" s="42">
+        <v>0</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="38">
+      <c r="A17" s="36">
         <v>1995</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="30">
         <v>100</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="32">
         <v>32</v>
       </c>
-      <c r="D17" s="47">
-        <v>0</v>
-      </c>
-      <c r="E17" s="48">
-        <v>0</v>
-      </c>
-      <c r="H17" s="25" t="s">
+      <c r="D17" s="41">
+        <v>0</v>
+      </c>
+      <c r="E17" s="42">
+        <v>0</v>
+      </c>
+      <c r="H17" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="38">
+      <c r="A18" s="36">
         <v>1996</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="30">
         <v>110</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="32">
         <v>40</v>
       </c>
-      <c r="D18" s="47">
-        <v>0</v>
-      </c>
-      <c r="E18" s="48">
-        <v>0</v>
-      </c>
-      <c r="H18" s="27" t="s">
+      <c r="D18" s="41">
+        <v>0</v>
+      </c>
+      <c r="E18" s="42">
+        <v>0</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+      <c r="A19" s="36">
         <v>1997</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="30">
         <v>120</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="32">
         <v>48</v>
       </c>
-      <c r="D19" s="47">
-        <v>0</v>
-      </c>
-      <c r="E19" s="48">
-        <v>0</v>
-      </c>
-      <c r="H19" s="27" t="s">
+      <c r="D19" s="41">
+        <v>0</v>
+      </c>
+      <c r="E19" s="42">
+        <v>0</v>
+      </c>
+      <c r="H19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="38">
+      <c r="A20" s="36">
         <v>1998</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="30">
         <v>130</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="32">
         <v>56</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="34">
         <v>6</v>
       </c>
-      <c r="E20" s="48">
-        <v>0</v>
-      </c>
-      <c r="H20" s="27" t="s">
+      <c r="E20" s="42">
+        <v>0</v>
+      </c>
+      <c r="H20" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="38">
+      <c r="A21" s="36">
         <v>1999</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="30">
         <v>140</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="32">
         <v>64</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="35">
         <v>12</v>
       </c>
-      <c r="E21" s="48">
-        <v>0</v>
-      </c>
-      <c r="H21" s="27" t="s">
+      <c r="E21" s="42">
+        <v>0</v>
+      </c>
+      <c r="H21" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
+      <c r="A22" s="36">
         <v>2000</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="30">
         <v>150</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="32">
         <v>72</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D22" s="35">
         <v>18</v>
       </c>
-      <c r="E22" s="48">
-        <v>0</v>
-      </c>
-      <c r="H22" s="29" t="s">
+      <c r="E22" s="42">
+        <v>0</v>
+      </c>
+      <c r="H22" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="38">
+      <c r="A23" s="36">
         <v>2001</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="30">
         <v>160</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="32">
         <v>80</v>
       </c>
-      <c r="D23" s="37">
+      <c r="D23" s="35">
         <v>24</v>
       </c>
-      <c r="E23" s="48">
-        <v>0</v>
-      </c>
-      <c r="H23" s="13" t="s">
+      <c r="E23" s="42">
+        <v>0</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="38">
+      <c r="A24" s="36">
         <v>2002</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="30">
         <v>170</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="32">
         <v>88</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="35">
         <v>30</v>
       </c>
-      <c r="E24" s="48">
-        <v>0</v>
-      </c>
-      <c r="H24" s="13" t="s">
+      <c r="E24" s="42">
+        <v>0</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
     </row>
     <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
+      <c r="A25" s="36">
         <v>2003</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="30">
         <v>180</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="33">
         <v>96</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="35">
         <v>36</v>
       </c>
-      <c r="E25" s="48">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15" t="s">
+      <c r="E25" s="42">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="38">
+      <c r="A26" s="36">
         <v>2004</v>
       </c>
-      <c r="B26" s="40">
+      <c r="B26" s="38">
         <v>190</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="38">
         <v>104</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="38">
         <v>42</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="38">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="38">
+      <c r="A27" s="36">
         <v>2005</v>
       </c>
-      <c r="B27" s="41">
+      <c r="B27" s="39">
         <v>200</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="39">
         <v>112</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="39">
         <v>48</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="38">
+      <c r="A28" s="36">
         <v>2006</v>
       </c>
-      <c r="B28" s="41">
+      <c r="B28" s="39">
         <v>210</v>
       </c>
-      <c r="C28" s="41">
+      <c r="C28" s="39">
         <v>120</v>
       </c>
-      <c r="D28" s="41">
+      <c r="D28" s="39">
         <v>54</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="39">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="38">
+      <c r="A29" s="36">
         <v>2007</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="39">
         <v>220</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="39">
         <v>128</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="39">
         <v>60</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="38">
+      <c r="A30" s="36">
         <v>2008</v>
       </c>
-      <c r="B30" s="41">
+      <c r="B30" s="39">
         <v>230</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="39">
         <v>136</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="39">
         <v>66</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="39">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="37">
         <v>2009</v>
       </c>
-      <c r="B31" s="42">
+      <c r="B31" s="40">
         <v>240</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="40">
         <v>144</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="40">
         <v>72</v>
       </c>
-      <c r="E31" s="42">
+      <c r="E31" s="40">
         <v>24</v>
       </c>
     </row>

</xml_diff>